<commit_message>
add exclusion criteria for serious disabilities
</commit_message>
<xml_diff>
--- a/Documentation/variable name propagation spreadsheet.xlsx
+++ b/Documentation/variable name propagation spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/OneDrive/TVAttention/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="11_F07C26DA1B894F6F3218D72ABE48C41C51C2C9E1" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{958E5466-6CB2-B644-A3F0-66F9DD50B46E}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="11_F07C26DA1B894F6F3218D72ABE48C41C51C2C9E1" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{345F92FD-FBDA-D449-88F1-8BEEA148F77A}"/>
   <bookViews>
     <workbookView xWindow="8280" yWindow="1060" windowWidth="25040" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="410">
   <si>
     <t xml:space="preserve">BPI: CH HAS DIFF CONCENTRATING </t>
   </si>
@@ -1250,13 +1250,31 @@
   </si>
   <si>
     <t>Variables from NLSY79 (National Longitudinal Survey of Youth 1979) dataset</t>
+  </si>
+  <si>
+    <t>Crippled</t>
+  </si>
+  <si>
+    <t>C0594700</t>
+  </si>
+  <si>
+    <t>C0813700</t>
+  </si>
+  <si>
+    <t>C1003700</t>
+  </si>
+  <si>
+    <t>C1207400</t>
+  </si>
+  <si>
+    <t>HEALTH: CHILD IS CRIPPLED OR HAS ORTHOPEDIC HANDICAP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1359,6 +1377,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1808,7 +1832,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1945,6 +1969,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="405">
@@ -2657,10 +2684,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y125"/>
+  <dimension ref="A1:Y126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="T103" sqref="T103:U103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -5944,241 +5971,263 @@
       </c>
       <c r="Y102" s="20"/>
     </row>
-    <row r="103" spans="1:25" s="44" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="16" t="s">
+    <row r="103" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="B103" s="32" t="s">
+        <v>409</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="G103" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="I103" s="20"/>
+      <c r="L103" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="M103" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="N103" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="Q103" s="20"/>
+      <c r="T103" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="U103" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="Y103" s="20"/>
+    </row>
+    <row r="104" spans="1:25" s="44" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="16" t="s">
         <v>384</v>
       </c>
-      <c r="B103" s="42" t="s">
+      <c r="B104" s="42" t="s">
         <v>387</v>
       </c>
-      <c r="C103" s="41"/>
-      <c r="D103" s="15" t="s">
+      <c r="C104" s="41"/>
+      <c r="D104" s="15" t="s">
         <v>390</v>
       </c>
-      <c r="E103" s="15" t="s">
+      <c r="E104" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="F103" s="15" t="s">
+      <c r="F104" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="G103" s="15" t="s">
+      <c r="G104" s="15" t="s">
         <v>393</v>
       </c>
-      <c r="H103" s="16"/>
-      <c r="I103" s="24"/>
-      <c r="J103" s="16"/>
-      <c r="K103" s="16"/>
-      <c r="L103" s="15" t="s">
+      <c r="H104" s="16"/>
+      <c r="I104" s="24"/>
+      <c r="J104" s="16"/>
+      <c r="K104" s="16"/>
+      <c r="L104" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="M103" s="15" t="s">
+      <c r="M104" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="N103" s="15" t="s">
+      <c r="N104" s="15" t="s">
         <v>393</v>
       </c>
-      <c r="O103" s="16"/>
-      <c r="P103" s="16"/>
-      <c r="Q103" s="24"/>
-      <c r="R103" s="16"/>
-      <c r="S103" s="16"/>
-      <c r="T103" s="15" t="s">
+      <c r="O104" s="16"/>
+      <c r="P104" s="16"/>
+      <c r="Q104" s="24"/>
+      <c r="R104" s="16"/>
+      <c r="S104" s="16"/>
+      <c r="T104" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="U103" s="15" t="s">
+      <c r="U104" s="15" t="s">
         <v>393</v>
       </c>
-      <c r="V103" s="41"/>
-      <c r="W103" s="41"/>
-      <c r="X103" s="41"/>
-      <c r="Y103" s="43"/>
-    </row>
-    <row r="104" spans="1:25" s="44" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="50" t="s">
+      <c r="V104" s="41"/>
+      <c r="W104" s="41"/>
+      <c r="X104" s="41"/>
+      <c r="Y104" s="43"/>
+    </row>
+    <row r="105" spans="1:25" s="44" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="50" t="s">
         <v>403</v>
       </c>
-      <c r="B104" s="51"/>
-      <c r="D104" s="9"/>
-      <c r="E104" s="9"/>
-      <c r="F104" s="9"/>
-      <c r="G104" s="9"/>
-      <c r="H104" s="6"/>
-      <c r="I104" s="20"/>
-      <c r="J104" s="6"/>
-      <c r="K104" s="6"/>
-      <c r="L104" s="9"/>
-      <c r="M104" s="9"/>
-      <c r="N104" s="9"/>
-      <c r="O104" s="6"/>
-      <c r="P104" s="6"/>
-      <c r="Q104" s="20"/>
-      <c r="R104" s="6"/>
-      <c r="S104" s="6"/>
-      <c r="T104" s="9"/>
-      <c r="U104" s="9"/>
-      <c r="Y104" s="52"/>
-    </row>
-    <row r="105" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="9"/>
-      <c r="C105" s="9"/>
-      <c r="D105" s="10"/>
+      <c r="B105" s="51"/>
+      <c r="D105" s="9"/>
       <c r="E105" s="9"/>
       <c r="F105" s="9"/>
       <c r="G105" s="9"/>
+      <c r="H105" s="6"/>
       <c r="I105" s="20"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="9"/>
       <c r="M105" s="9"/>
       <c r="N105" s="9"/>
+      <c r="O105" s="6"/>
+      <c r="P105" s="6"/>
       <c r="Q105" s="20"/>
-      <c r="Y105" s="20"/>
+      <c r="R105" s="6"/>
+      <c r="S105" s="6"/>
+      <c r="T105" s="9"/>
+      <c r="U105" s="9"/>
+      <c r="Y105" s="52"/>
     </row>
     <row r="106" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="B106" s="9" t="s">
-        <v>261</v>
-      </c>
+      <c r="B106" s="9"/>
       <c r="C106" s="9"/>
       <c r="D106" s="10"/>
       <c r="E106" s="9"/>
-      <c r="F106" s="9" t="s">
-        <v>260</v>
-      </c>
+      <c r="F106" s="9"/>
       <c r="G106" s="9"/>
       <c r="I106" s="20"/>
-      <c r="M106" s="9" t="s">
-        <v>260</v>
-      </c>
+      <c r="M106" s="9"/>
       <c r="N106" s="9"/>
       <c r="Q106" s="20"/>
-      <c r="T106" s="6" t="s">
-        <v>260</v>
-      </c>
       <c r="Y106" s="20"/>
     </row>
     <row r="107" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B107" s="9"/>
+      <c r="A107" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>261</v>
+      </c>
       <c r="C107" s="9"/>
       <c r="D107" s="10"/>
       <c r="E107" s="9"/>
-      <c r="F107" s="9"/>
+      <c r="F107" s="9" t="s">
+        <v>260</v>
+      </c>
       <c r="G107" s="9"/>
       <c r="I107" s="20"/>
-      <c r="M107" s="9"/>
+      <c r="M107" s="9" t="s">
+        <v>260</v>
+      </c>
       <c r="N107" s="9"/>
       <c r="Q107" s="20"/>
+      <c r="T107" s="6" t="s">
+        <v>260</v>
+      </c>
       <c r="Y107" s="20"/>
     </row>
     <row r="108" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="B108" s="9" t="s">
-        <v>262</v>
-      </c>
+      <c r="B108" s="9"/>
       <c r="C108" s="9"/>
-      <c r="D108" s="10" t="s">
-        <v>265</v>
-      </c>
+      <c r="D108" s="10"/>
       <c r="E108" s="9"/>
       <c r="F108" s="9"/>
       <c r="G108" s="9"/>
       <c r="I108" s="20"/>
-      <c r="K108" s="6" t="s">
-        <v>265</v>
-      </c>
       <c r="M108" s="9"/>
       <c r="N108" s="9"/>
       <c r="Q108" s="20"/>
-      <c r="S108" s="6" t="s">
+      <c r="Y108" s="20"/>
+    </row>
+    <row r="109" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C109" s="9"/>
+      <c r="D109" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="Y108" s="20"/>
-    </row>
-    <row r="109" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B109" s="9"/>
-      <c r="C109" s="9"/>
-      <c r="D109" s="10"/>
       <c r="E109" s="9"/>
       <c r="F109" s="9"/>
       <c r="G109" s="9"/>
       <c r="I109" s="20"/>
+      <c r="K109" s="6" t="s">
+        <v>265</v>
+      </c>
       <c r="M109" s="9"/>
       <c r="N109" s="9"/>
       <c r="Q109" s="20"/>
+      <c r="S109" s="6" t="s">
+        <v>265</v>
+      </c>
       <c r="Y109" s="20"/>
     </row>
     <row r="110" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="6" t="s">
+      <c r="B110" s="9"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="10"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="9"/>
+      <c r="I110" s="20"/>
+      <c r="M110" s="9"/>
+      <c r="N110" s="9"/>
+      <c r="Q110" s="20"/>
+      <c r="Y110" s="20"/>
+    </row>
+    <row r="111" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="B110" s="9" t="s">
+      <c r="B111" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="C110" s="9"/>
-      <c r="D110" s="10" t="s">
+      <c r="C111" s="9"/>
+      <c r="D111" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="E110" s="9" t="s">
+      <c r="E111" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F110" s="28" t="s">
+      <c r="F111" s="28" t="s">
         <v>275</v>
       </c>
-      <c r="G110" s="28" t="s">
+      <c r="G111" s="28" t="s">
         <v>270</v>
       </c>
-      <c r="H110" s="25" t="s">
+      <c r="H111" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="I110" s="20"/>
-      <c r="L110" s="9" t="s">
+      <c r="I111" s="20"/>
+      <c r="L111" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="M110" s="9" t="s">
+      <c r="M111" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="N110" s="12" t="s">
+      <c r="N111" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="O110" s="11" t="s">
+      <c r="O111" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="P110" s="11" t="s">
+      <c r="P111" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="Q110" s="20"/>
-      <c r="T110" s="9" t="s">
+      <c r="Q111" s="20"/>
+      <c r="T111" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="U110" s="9" t="s">
+      <c r="U111" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="V110" s="11" t="s">
+      <c r="V111" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="W110" s="11" t="s">
+      <c r="W111" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="X110" s="11" t="s">
+      <c r="X111" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="Y110" s="20"/>
-    </row>
-    <row r="111" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B111" s="9"/>
-      <c r="C111" s="9"/>
-      <c r="D111" s="10"/>
-      <c r="E111" s="9"/>
-      <c r="F111" s="9"/>
-      <c r="G111" s="9"/>
-      <c r="I111" s="20"/>
-      <c r="L111" s="9"/>
-      <c r="M111" s="9"/>
-      <c r="N111" s="9"/>
-      <c r="Q111" s="20"/>
-      <c r="T111" s="9"/>
-      <c r="U111" s="9"/>
       <c r="Y111" s="20"/>
     </row>
     <row r="112" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -6189,221 +6238,237 @@
       <c r="F112" s="9"/>
       <c r="G112" s="9"/>
       <c r="I112" s="20"/>
+      <c r="L112" s="9"/>
       <c r="M112" s="9"/>
       <c r="N112" s="9"/>
       <c r="Q112" s="20"/>
+      <c r="T112" s="9"/>
+      <c r="U112" s="9"/>
       <c r="Y112" s="20"/>
     </row>
-    <row r="113" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="6" t="s">
+    <row r="113" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B113" s="9"/>
+      <c r="C113" s="9"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="9"/>
+      <c r="F113" s="9"/>
+      <c r="G113" s="9"/>
+      <c r="I113" s="20"/>
+      <c r="M113" s="9"/>
+      <c r="N113" s="9"/>
+      <c r="Q113" s="20"/>
+      <c r="Y113" s="20"/>
+    </row>
+    <row r="114" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A114" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="B113" s="32" t="s">
+      <c r="B114" s="32" t="s">
         <v>291</v>
       </c>
-      <c r="C113" s="9"/>
-      <c r="D113" s="37" t="s">
+      <c r="C114" s="9"/>
+      <c r="D114" s="37" t="s">
         <v>292</v>
       </c>
-      <c r="E113" s="37" t="s">
+      <c r="E114" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="F113" s="37" t="s">
+      <c r="F114" s="37" t="s">
         <v>294</v>
       </c>
-      <c r="G113" s="37" t="s">
+      <c r="G114" s="37" t="s">
         <v>295</v>
       </c>
-      <c r="H113" s="37" t="s">
+      <c r="H114" s="37" t="s">
         <v>297</v>
       </c>
-      <c r="I113" s="29"/>
-      <c r="L113" s="39" t="s">
+      <c r="I114" s="29"/>
+      <c r="L114" s="39" t="s">
         <v>293</v>
       </c>
-      <c r="M113" s="39" t="s">
+      <c r="M114" s="39" t="s">
         <v>294</v>
       </c>
-      <c r="N113" s="39" t="s">
+      <c r="N114" s="39" t="s">
         <v>295</v>
       </c>
-      <c r="O113" s="39" t="s">
+      <c r="O114" s="39" t="s">
         <v>297</v>
       </c>
-      <c r="P113" s="39" t="s">
+      <c r="P114" s="39" t="s">
         <v>298</v>
       </c>
-      <c r="Q113" s="29"/>
-      <c r="T113" s="39" t="s">
+      <c r="Q114" s="29"/>
+      <c r="T114" s="39" t="s">
         <v>294</v>
       </c>
-      <c r="U113" s="39" t="s">
+      <c r="U114" s="39" t="s">
         <v>295</v>
       </c>
-      <c r="V113" s="39" t="s">
+      <c r="V114" s="39" t="s">
         <v>297</v>
       </c>
-      <c r="W113" s="39" t="s">
+      <c r="W114" s="39" t="s">
         <v>298</v>
       </c>
-      <c r="X113" s="39" t="s">
+      <c r="X114" s="39" t="s">
         <v>299</v>
       </c>
-      <c r="Y113" s="20"/>
-    </row>
-    <row r="114" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B114" s="32" t="s">
+      <c r="Y114" s="20"/>
+    </row>
+    <row r="115" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B115" s="32" t="s">
         <v>300</v>
       </c>
-      <c r="C114" s="9"/>
-      <c r="D114" s="38" t="s">
+      <c r="C115" s="9"/>
+      <c r="D115" s="38" t="s">
         <v>301</v>
       </c>
-      <c r="E114" s="38" t="s">
+      <c r="E115" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="F114" s="37" t="s">
+      <c r="F115" s="37" t="s">
         <v>302</v>
       </c>
-      <c r="G114" s="37" t="s">
+      <c r="G115" s="37" t="s">
         <v>303</v>
       </c>
-      <c r="H114" s="37" t="s">
+      <c r="H115" s="37" t="s">
         <v>304</v>
       </c>
-      <c r="I114" s="29"/>
-      <c r="L114" s="38" t="s">
+      <c r="I115" s="29"/>
+      <c r="L115" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="M114" s="38" t="s">
+      <c r="M115" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="N114" s="39" t="s">
+      <c r="N115" s="39" t="s">
         <v>303</v>
       </c>
-      <c r="O114" s="39" t="s">
+      <c r="O115" s="39" t="s">
         <v>304</v>
       </c>
-      <c r="P114" s="39" t="s">
+      <c r="P115" s="39" t="s">
         <v>305</v>
       </c>
-      <c r="Q114" s="29"/>
-      <c r="T114" s="38" t="s">
+      <c r="Q115" s="29"/>
+      <c r="T115" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="U114" s="38" t="s">
+      <c r="U115" s="38" t="s">
         <v>303</v>
       </c>
-      <c r="V114" s="39" t="s">
+      <c r="V115" s="39" t="s">
         <v>304</v>
       </c>
-      <c r="W114" s="39" t="s">
+      <c r="W115" s="39" t="s">
         <v>305</v>
       </c>
-      <c r="X114" s="39" t="s">
+      <c r="X115" s="39" t="s">
         <v>306</v>
       </c>
-      <c r="Y114" s="20"/>
-    </row>
-    <row r="115" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B115" s="9"/>
-      <c r="C115" s="9"/>
-      <c r="D115" s="10"/>
-      <c r="E115" s="9"/>
-      <c r="F115" s="9"/>
-      <c r="G115" s="9"/>
-      <c r="I115" s="20"/>
-      <c r="M115" s="9"/>
-      <c r="N115" s="9"/>
-      <c r="Q115" s="20"/>
       <c r="Y115" s="20"/>
     </row>
-    <row r="116" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="6" t="s">
+    <row r="116" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B116" s="9"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="10"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="9"/>
+      <c r="I116" s="20"/>
+      <c r="M116" s="9"/>
+      <c r="N116" s="9"/>
+      <c r="Q116" s="20"/>
+      <c r="Y116" s="20"/>
+    </row>
+    <row r="117" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A117" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="B116" s="32" t="s">
+      <c r="B117" s="32" t="s">
         <v>308</v>
       </c>
-      <c r="C116" s="9"/>
-      <c r="D116" s="37" t="s">
+      <c r="C117" s="9"/>
+      <c r="D117" s="37" t="s">
         <v>309</v>
       </c>
-      <c r="E116" s="37" t="s">
+      <c r="E117" s="37" t="s">
         <v>310</v>
       </c>
-      <c r="F116" s="37" t="s">
+      <c r="F117" s="37" t="s">
         <v>311</v>
       </c>
-      <c r="G116" s="37" t="s">
+      <c r="G117" s="37" t="s">
         <v>312</v>
       </c>
-      <c r="H116" s="37" t="s">
+      <c r="H117" s="37" t="s">
         <v>313</v>
       </c>
-      <c r="I116" s="29"/>
-      <c r="L116" s="39" t="s">
+      <c r="I117" s="29"/>
+      <c r="L117" s="39" t="s">
         <v>310</v>
       </c>
-      <c r="M116" s="39" t="s">
+      <c r="M117" s="39" t="s">
         <v>311</v>
       </c>
-      <c r="N116" s="39" t="s">
+      <c r="N117" s="39" t="s">
         <v>312</v>
       </c>
-      <c r="O116" s="39" t="s">
+      <c r="O117" s="39" t="s">
         <v>313</v>
       </c>
-      <c r="P116" s="39" t="s">
+      <c r="P117" s="39" t="s">
         <v>314</v>
       </c>
-      <c r="Q116" s="29"/>
-      <c r="T116" s="39" t="s">
+      <c r="Q117" s="29"/>
+      <c r="T117" s="39" t="s">
         <v>311</v>
       </c>
-      <c r="U116" s="39" t="s">
+      <c r="U117" s="39" t="s">
         <v>312</v>
       </c>
-      <c r="V116" s="39" t="s">
+      <c r="V117" s="39" t="s">
         <v>313</v>
       </c>
-      <c r="W116" s="39" t="s">
+      <c r="W117" s="39" t="s">
         <v>314</v>
       </c>
-      <c r="X116" s="39" t="s">
+      <c r="X117" s="39" t="s">
         <v>315</v>
       </c>
-      <c r="Y116" s="20"/>
-    </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A117" s="16"/>
-      <c r="B117" s="16"/>
-      <c r="C117" s="16"/>
-      <c r="D117" s="16"/>
-      <c r="E117" s="16"/>
-      <c r="F117" s="16"/>
-      <c r="G117" s="16"/>
-      <c r="H117" s="16"/>
-      <c r="I117" s="24"/>
-      <c r="J117" s="16"/>
-      <c r="K117" s="16"/>
-      <c r="L117" s="16"/>
-      <c r="M117" s="16"/>
-      <c r="N117" s="16"/>
-      <c r="O117" s="16"/>
-      <c r="P117" s="16"/>
-      <c r="Q117" s="24"/>
-      <c r="R117" s="16"/>
-      <c r="S117" s="16"/>
-      <c r="T117" s="16"/>
-      <c r="U117" s="16"/>
-      <c r="V117" s="16"/>
-      <c r="W117" s="16"/>
-      <c r="X117" s="16"/>
-      <c r="Y117" s="24"/>
-    </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="L125" s="13"/>
+      <c r="Y117" s="20"/>
+    </row>
+    <row r="118" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A118" s="16"/>
+      <c r="B118" s="16"/>
+      <c r="C118" s="16"/>
+      <c r="D118" s="16"/>
+      <c r="E118" s="16"/>
+      <c r="F118" s="16"/>
+      <c r="G118" s="16"/>
+      <c r="H118" s="16"/>
+      <c r="I118" s="24"/>
+      <c r="J118" s="16"/>
+      <c r="K118" s="16"/>
+      <c r="L118" s="16"/>
+      <c r="M118" s="16"/>
+      <c r="N118" s="16"/>
+      <c r="O118" s="16"/>
+      <c r="P118" s="16"/>
+      <c r="Q118" s="24"/>
+      <c r="R118" s="16"/>
+      <c r="S118" s="16"/>
+      <c r="T118" s="16"/>
+      <c r="U118" s="16"/>
+      <c r="V118" s="16"/>
+      <c r="W118" s="16"/>
+      <c r="X118" s="16"/>
+      <c r="Y118" s="24"/>
+    </row>
+    <row r="126" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="L126" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>